<commit_message>
bottoni ma sono brutti
</commit_message>
<xml_diff>
--- a/Descrizione_Luoghi.xlsx
+++ b/Descrizione_Luoghi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{440E64A7-5299-417F-B905-5AFA614C20F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4B39F0-A4C1-400E-9F3B-B81ECDF7EAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C859E47D-5930-4D37-A0D3-BED1110D8150}"/>
   </bookViews>
@@ -612,13 +612,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A8483D-001F-43E4-850C-193FC62F6C85}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="118.6640625" customWidth="1"/>
+    <col min="2" max="2" width="123.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
dicono di noi chiedi a chat di recensire
</commit_message>
<xml_diff>
--- a/Descrizione_Luoghi.xlsx
+++ b/Descrizione_Luoghi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E38B19D-4F24-4782-9B45-B429ADE4D2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31550001-751C-444D-9CC7-FEDBE8F6E2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C859E47D-5930-4D37-A0D3-BED1110D8150}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
   <si>
     <t>I1</t>
   </si>
@@ -263,6 +263,189 @@
   <si>
     <t>Un’intuizione geniale a pochi passi dal Pantheon che non potete assolutamente perdervi. Che sia per un aperitivo, un pranzo o una cena veloci, grazie ad una conveniente offerta 
 (aperipizza) a 10€ potrete avere un drink e un tagliere di pizza “alla romana” a vari gusti. €</t>
+  </si>
+  <si>
+    <t>Tutto il mangiare e bere della Sardegna nel cuore di Roma, enoteca fornitissima, prodotti ricercati e cura dei particolari. Un aperitivo unico nel suo genere. Prezzi un po' alti per lo 
+standard aperitivo. €€€</t>
+  </si>
+  <si>
+    <t>Bistrot turistico zona circo massimo adatto a una pausa veloce. €</t>
+  </si>
+  <si>
+    <t>Bar di fronte al Circo Massimo sulla via dei Cerchi. Arredato in stile moderno con dipinti e quadri coloratissimi è un punto di ristoro efficace e valido. €</t>
+  </si>
+  <si>
+    <t>Aperitivi, Apericena, Cocktail bar, Giardino e Spazio per eventi di ogni genere. Il punto forte è sicuro la location. €€€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locale rustico con archi in pietra, che offre una vasta scelta di vini, formaggi e salumi. Hanno tantissimi tipi di birra anche quelle artigianali e l'aperitivo a buffet è molto economico. </t>
+  </si>
+  <si>
+    <t>Dal giorno alla notte: bar &amp; bistrot, american breakfast, light lunch, aperitivo, cena e dopocena in una delle piazze più suggestive della Capitale, nel cuore di Trastevere. A 10€ ti portano 
+un tagliere pienissimo e un drink, assolutamente conveniente.  €</t>
+  </si>
+  <si>
+    <t>Il quarto ristorante del brand Polpetta sorge nel cuore di uno dei quartieri più storici in assoluto a Roma: Trastevere. Inoltre per coronare al meglio il tutto è stato scelto un luogo 
+ben preciso… Gli storici Giardini della Fornarina di Raffaello, luogo magico e suggestivo in grado di rievocare la tradizione romana. Come poter resistere a un aperitivo a base di 
+polpette di ogni genere? €</t>
+  </si>
+  <si>
+    <t>Wine bar ricoperto di edera, con muri in pietra a vista e legno scuro, che serve piatti tipici locali a lume di candela. €</t>
+  </si>
+  <si>
+    <t>Vivace bar con terrazza animata, dove gustare cocktail e aperitivi tra lampadari e arte moderna. €</t>
+  </si>
+  <si>
+    <t>Al n. 13 di Borgo Pio c'è un posto delizioso dove trascorrere un po' di tempo in tranquillità, in un'atmosfera intima ed accogliente. Ideale per un aperitivo e quattro chiacchiere in 
+compagnia, ti coinvolge anche con degli ottimi stuzzichini e qualche piatto di ottima fattura. Posto ben lontano dalle trappole per turisti in quella zona.  €€</t>
+  </si>
+  <si>
+    <t>Winebar, birreria, cocktail bar e libreria ma anche un vero e proprio emporio del tè nel cuore di Roma, che si trasforma per chiunque lo visiti in un’oasi di relax. Taglieri, bruschette e 
+stuzzichini per l’aperitivo comodamente seduti al bancone o ai tavolini negli angoli etnici. €</t>
+  </si>
+  <si>
+    <t>Una lunga lista di cocktail e vini regionali offerti in un elegante bar in stile Art Déco con una terrazza panoramica. €€€</t>
+  </si>
+  <si>
+    <t>Locale sofisticato disposto su due livelli con espresso, cocktail e piatti da bar, oltre a un programma regolare di concerti jazz. €€</t>
+  </si>
+  <si>
+    <t>Non è un pub, non è un bistrot e non è una trattoria, ma in realtà è un mix di tutto questo. Non hanno una vera e propria formula aperitivo ma ti danno un tagliere con degli assaggi 
+di tutto il menu €€</t>
+  </si>
+  <si>
+    <t>Primo TARTARE BAR d’Italia, un locale intimo con pochi coperti, specializzato in crudi di carne e di pesce, una buona selezione di vini ed un cocktail bar con homemade cocktails, 
+tutto a gestione familiare, nella splendida cornice di piazza Sallustio</t>
+  </si>
+  <si>
+    <t>Da febbraio 2019 il bar del St. Regis si è rinnovato da cima a fondo, trasformandosi in LUMEN – Cocktail &amp; Cuisine, spazio dedicato al cibo e al beverage, attivo praticamente in ogni 
+momento del giorno, dalla colazione al drink di fine cena.  €€€</t>
+  </si>
+  <si>
+    <t>Ottimo aperitivo a 8€ con patatine focacce e pizzette, buono per due, drink ottimi, locale perfetto perciò per un aperitivo a Trastevere fra amici. Locale con arredamento particolare 
+e bella musica, location davanti a piazza Trilussa. €</t>
+  </si>
+  <si>
+    <t>A pochi metri dal Colosseo, proprio sotto la sua ombra, in un luogo meraviglioso per la panoramica dell’Anfiteatro Flavio, si trova il Coming Out. Punto di aggregazione e ritrovo 
+della comunità LGBTQ di Roma.  Propongono formula aperitivo a 14€.  €</t>
+  </si>
+  <si>
+    <t>A pochi passi dal Colosseo e da San Giovanni, il lunch cafè Colosseum Bar, oltre al servizio bar, mette a vostra disposizione un ricco ventaglio di soluzioni sfiziose per una vera 
+pausa di gusto nel cuore di Roma €€€</t>
+  </si>
+  <si>
+    <t>Aperitivo affacciati sul Colosseo al tramonto, non ha prezzo. Drink ricercati con prodotti particolari e di qualità. Terrazza dell'hotel Palazzo Manfredi. Prezzi in linea con la location. €€€€</t>
+  </si>
+  <si>
+    <t>Vicino al Colosseo e alle vie più vivaci, un angolo di pace e buon gusto con una terrazza che offre vista e refrigerio nelle calde notti romane. €€€</t>
+  </si>
+  <si>
+    <t>Tranquilla caffetteria all'aperto tra gli alberi, che serve caffè, spuntini e cocktail. €</t>
+  </si>
+  <si>
+    <t>Storico bar nel cuore di Testaccio, nel quale la tradizione si unisce a un ambiente moderno e innova €€</t>
+  </si>
+  <si>
+    <t>Il gianfornaio è una sicurezza per ogni momento della giornata:  una colazione veloce prima del lavoro o di una partenza, una mattinata di studio con una tazza di caffè, un pranzo 
+tra colleghi o un aperitivo tra vecchi amici. €€</t>
+  </si>
+  <si>
+    <t>400 mq divisi in ristorante, bar/caffetteria, grill, loft garden, cucina a vista e materiali rudi, come il grande bancone in pietra a spacco, con spazio macelleria, che quasi fuoriesce sul 
+marciapiede. Happy hour dalle 18 che con 10€ comprende un drink ed accesso libero al buffet, 8 metri quadri di bancone con piatti freddi e caldi, espressi dalla cucina €</t>
+  </si>
+  <si>
+    <t>Casa Manfredi, una delle pasticcerie più apprezzate di Roma in cui fermarsi anche per un aperitivo. Raffinate e gustose preparazioni di Alta Pasticceria realizzate con i prodotti Agrimontana &amp; accompagnate dalle Bollicine di Montagna ROTARI Trendo DOC!
+Ogni giorno dalle 18 alle 21.. sulle Sponde di Viale Aventino. €€€</t>
+  </si>
+  <si>
+    <t>Negli spazi della Galleria D'Arte del Palazzo Pamphilj, al quarto piano, è presente Terrazza Borromini, capace di incorniciare una delle viste più suggestiva della celebre Piazza Navona.
+Per un aperitivo al tramonto in una location superba. €€€</t>
+  </si>
+  <si>
+    <t>Rooftop bar nel cuore a Roma, a tema Spritz. Drink list a base bollicine, musica e tapas, panorama suggestivo. Se siete amanti dello spritz non potete perdervelo. €€</t>
+  </si>
+  <si>
+    <t>Forno/bar Trevi dai mille gusti per un aperitivo accompagnato da un tagliere perfetto con vista sulla magnifica Fontana di Trevi. €€</t>
+  </si>
+  <si>
+    <t>Il nome è la descrzione di questo magico posto. I loro taglieri sono inegugliabili! Prodotti tipici toscani di una qualità ottima. €€</t>
+  </si>
+  <si>
+    <t>Wine bar intimo e accogliente che serve panini, oltre a taglieri di salumi, formaggi e bruschette. €</t>
+  </si>
+  <si>
+    <t>Locale situato nell'interessante cornice di Piazza Cola di Rienzo, ampio lo spazio esterno, personale alla mano e servizio rapido... buona lista di cocktails che in caso di scelta della 
+formula aperitivo completo, verrà accompagnato da una piramide di sfiziosità composta da salumi, formaggi e pizza al costo di 15€.  €</t>
+  </si>
+  <si>
+    <t>Piccolo chioschetto di strada in stile bohémien con tavoli all'aperto che offre cocktail, vini naturali e birre artigianali, oltre a caffè. €</t>
+  </si>
+  <si>
+    <t>Panineria trendy con ingredienti vegetariani e condimenti creativi. €€</t>
+  </si>
+  <si>
+    <t>Un localino in pieno centro a Roma, alle spalle della metro Cavour. Piccola location ma molto caratteristica ed accogliente. Il punto forte è il un tagliere Freeda che solo 
+con quello potete dire sto bene. €</t>
+  </si>
+  <si>
+    <t>Un café esclusivo, all’interno dell’Apollo Boutique Hotel di Roma, a vostra disposizione dalla colazione all’aperitivo. Dalle 18:30 alle 21:00 BUFFET ILLIMITATO + BEVANDA = 15 euro. €</t>
+  </si>
+  <si>
+    <t>Il Maritozzo, uno dei simboli della cucina romana, ma in versione salata. Sicuramente un aperitivo diverso dell'ordinario. €€</t>
+  </si>
+  <si>
+    <t>Enoteca con possibilità di degustare prodotti tipici di provenienti dal Cilento, vini di qualità e prodotti ricercati. Aperitivi, cena, degustazioni, corsi sul vino e cultura. €€</t>
+  </si>
+  <si>
+    <t>Il punto di forza principale di questo ristorante poco distante da Cola di Rienzo è senza dubbio la terrazza con vista sui tetti di Roma. €€€</t>
+  </si>
+  <si>
+    <t>Ristorante contemporaneo dall’atmosfera parigina e design newyorkese che dal pranzo al dopocena seleziona soltanto il meglio, puntando su eleganza e socialità. €€€</t>
+  </si>
+  <si>
+    <t>Sobrio bar/bistrot eclettico che serve stuzzichini e cocktail classici, oltre a una selezione di vini e birre. €€</t>
+  </si>
+  <si>
+    <t>Aperitivi a buffet in piccolo locale dalle pareti colorate con mensole di vetro all'interno di cornici dorate. Ampio spazio esterno proprio su piazza cola di rienzo €</t>
+  </si>
+  <si>
+    <t>Cocktail bar, vini e non solo, accompagnati da una selezione di prodotti gastronomici italiani ed iberici, in un ambiente che celebra le atmosfere, i colori e la musica di Cuba. €€</t>
+  </si>
+  <si>
+    <t>Idea molto sfiziosa, un locale che propone "cicchetti" a scelta dello chef, piccole "tapas" in stile Veneto preparate sull'estro del momento. Tre combinazioni tra cui scegliere 5/10/15 
+cicchetti. €€</t>
+  </si>
+  <si>
+    <t>Pub che serve hamburger, pasta, aperitivo e birra, con vista San Pietro, oltre a sport in TV. €€</t>
+  </si>
+  <si>
+    <t>Locale  in una zona molto tranquilla di Prati. Formula aperitivo che consiste in una bevanda e un piatto di stuzzichini ad 8 euro. €</t>
+  </si>
+  <si>
+    <t>Bar in una delle piazze storiche romane, tappa fissa per le pause pranzo di chi lavora in quella zona. €</t>
+  </si>
+  <si>
+    <t>Tonico Café  offre musica soft in un ambiente confortevole in un esclusivo dehor esterno con deliziose tapas per aperitivo. €€</t>
+  </si>
+  <si>
+    <t>Aperitivo di qualità a prezzi modici: oltre agli indispensabili stuzzichini un tagliere di salumi e formaggi di prima qualità accompagnati da pizza scrocchiarella e cocktail originali 
+(fatevi consigliare dal proprietario, che se ne inventa sempre uno nuovo!) €€</t>
+  </si>
+  <si>
+    <t>Un angolo verde nel cuore di roma dove cibo e cocktail si fondono con la musica per creare l'atmosfera giusta. €€</t>
+  </si>
+  <si>
+    <t>Cappuccino, tè inglese e spuntini leggeri in un caratteristico locale con mobili vintage e opere d'arte. Caratteristici aperitivi sia dolci che salati €€</t>
+  </si>
+  <si>
+    <t>Puoi scegliere la combinazione che preferisci fra oltre 100 snack diversi. Ogni box è unica, realizzata con prodotti freschi e materie prime di altissima qualità, in base alla stagionalità 
+e alla reperibilità dei prodotti. €€</t>
+  </si>
+  <si>
+    <t>Tutti i tipi di drink accompagnati dalle storiche tartine, dai nuovissimi crostini e da tantissime specialità gastromoniche di prima scelta. €€</t>
+  </si>
+  <si>
+    <t>Locale in cui puoi trovare prodotti italiani e di altre provenienze come il pregiatissimo prosciutto Iberico Pata Negra ed il prosciutto Serrano di qualità eccellente. €€</t>
   </si>
 </sst>
 </file>
@@ -304,13 +487,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -629,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A8483D-001F-43E4-850C-193FC62F6C85}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,7 +829,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -674,7 +853,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -682,7 +861,7 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
     </row>
@@ -690,7 +869,7 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -698,7 +877,7 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>73</v>
       </c>
     </row>
@@ -706,7 +885,7 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -714,7 +893,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -722,283 +901,448 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>